<commit_message>
feat: send order to admin
</commit_message>
<xml_diff>
--- a/files/Order.xlsx
+++ b/files/Order.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALSU\Desktop\eliana_price_server\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alsu\Desktop\eliana_price_server\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="12432"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Заказ" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -341,7 +341,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>